<commit_message>
added more tests and added Read me file
</commit_message>
<xml_diff>
--- a/data/expense-categorizer-sampledata.xlsx
+++ b/data/expense-categorizer-sampledata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pcadmin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rohit\Downloads\Categorize\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D246771D-9EC3-495A-AFD5-FA4E22F1AFDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B188BB-C185-4D30-8BDD-CB65896B4207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2BD9C4D4-046F-4D63-80DC-B08FB4114620}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2BD9C4D4-046F-4D63-80DC-B08FB4114620}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -149,10 +147,10 @@
     <t>“Doctor visit co-pay”</t>
   </si>
   <si>
-    <t>“” (empty description)</t>
-  </si>
-  <si>
     <t>“Taxi downtown”</t>
+  </si>
+  <si>
+    <t>“”</t>
   </si>
 </sst>
 </file>
@@ -547,20 +545,20 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="25" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="25" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -580,7 +578,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -600,7 +598,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -620,7 +618,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -640,7 +638,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -660,7 +658,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -680,7 +678,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -700,7 +698,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -720,7 +718,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -740,12 +738,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C10" s="4">
         <v>100</v>
@@ -760,12 +758,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" s="4">
         <v>18.5</v>
@@ -780,7 +778,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -800,7 +798,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -820,7 +818,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -840,7 +838,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -860,7 +858,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -880,7 +878,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -900,7 +898,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -920,7 +918,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -940,7 +938,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -960,7 +958,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>20</v>
       </c>

</xml_diff>